<commit_message>
last stand from last warrior
</commit_message>
<xml_diff>
--- a/DigSite/New Arcaism/uarm 2025 2/urgh.xlsx
+++ b/DigSite/New Arcaism/uarm 2025 2/urgh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitData\ArchaeologyJourney\DigSite\New Arcaism\uarm 2025 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83F8499-8908-4B9D-BAE9-882FE262F8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702F92E2-89FB-4301-A3E4-85990D4D9767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="60" windowWidth="10395" windowHeight="10665" activeTab="1" xr2:uid="{1E955969-53D8-4BFC-8A4C-F24E13D91194}"/>
   </bookViews>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,6 +1710,9 @@
       <c r="D28">
         <v>15</v>
       </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">

</xml_diff>